<commit_message>
cleaned up xlsx organization and code
</commit_message>
<xml_diff>
--- a/exports/excel/calendar.xlsx
+++ b/exports/excel/calendar.xlsx
@@ -514,7 +514,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>7</c:v>
@@ -1706,7 +1706,7 @@
         <v>25</v>
       </c>
       <c r="B17">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2">

</xml_diff>